<commit_message>
Minor updates and additions
</commit_message>
<xml_diff>
--- a/Courses/Computer-Modeling-and-IT/Computer-Modeling-and-IT-6-Class/10-Formulas-and-Functions/Resources/temperature.xlsx
+++ b/Courses/Computer-Modeling-and-IT/Computer-Modeling-and-IT-6-Class/10-Formulas-and-Functions/Resources/temperature.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vs project\GitHub\School-Programming\Courses\Computer-Modeling-and-IT\Computer-Modeling-and-IT-6-Class\10-Formulas-and-Functions\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrinamehandzhiyska/Documents/GitHub/School-Programming/Courses/Computer-Modeling-and-IT/Computer-Modeling-and-IT-6-Class/10-Formulas-and-Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33893BF-CEAB-9E45-9CB8-36DD2A6F4D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
     <numFmt numFmtId="165" formatCode="0\°\C"/>
@@ -90,11 +91,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,33 +375,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -420,463 +421,463 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>45209</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>17</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>45209</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>45210</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>15</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>45210</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>45211</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>14</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>45211</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>13</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>45212</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>15</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>45212</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>15</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>45213</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>13</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>45213</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>45214</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>17</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>45214</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>45215</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>11</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>45215</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>45216</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>10</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>45216</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>45217</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>45217</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>45218</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>45218</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>45219</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>20</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>45219</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>45220</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>19</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>45220</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>45221</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>13</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>45221</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>45222</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>16</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>45222</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>45223</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>17</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>45223</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>45224</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>11</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>45224</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>45225</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>10</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>45225</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>45226</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>14</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>45226</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>45227</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>15</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>45227</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>45228</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>15</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>45228</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>45229</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>17</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>45229</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>45230</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>12</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>45230</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>45231</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>11</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>45231</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>12.7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>45232</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>14</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>45232</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>45233</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>14</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>45233</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>45234</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>15</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>45234</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>45235</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>16</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>45235</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>45236</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>16</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>45236</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>45237</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>17</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>45237</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>45238</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>10</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>45238</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>45239</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>8</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>45239</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>45240</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>6</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>45240</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>6</v>
       </c>
     </row>

</xml_diff>